<commit_message>
DDL DML e DQL e inicio da documentacao
</commit_message>
<xml_diff>
--- a/OpFlix/MER/M_Diagrama_RaulScapin_Fisico.xlsx
+++ b/OpFlix/MER/M_Diagrama_RaulScapin_Fisico.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20348"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E86D5D-2B2E-4B7D-A46C-EC6E49D0AE7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF851327-2DEE-4934-B86D-FD7307702DB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
   <si>
     <t>Usuarios</t>
   </si>
@@ -199,36 +199,9 @@
     <t>ra@gmail.com</t>
   </si>
   <si>
-    <t>Joice</t>
-  </si>
-  <si>
-    <t>jo@gmail.com</t>
-  </si>
-  <si>
-    <t>Joel</t>
-  </si>
-  <si>
-    <t>jojo@gmail.com</t>
-  </si>
-  <si>
-    <t>Airton</t>
-  </si>
-  <si>
-    <t>air@gmail.com</t>
-  </si>
-  <si>
-    <t>Bernando</t>
-  </si>
-  <si>
-    <t>be@gmail.com</t>
-  </si>
-  <si>
     <t>admin123</t>
   </si>
   <si>
-    <t>jo321123</t>
-  </si>
-  <si>
     <t>Os pequenos jovens em aventuras mirabolantes.</t>
   </si>
   <si>
@@ -298,10 +271,31 @@
     <t>Os pequeninos da Disney estao de volta.</t>
   </si>
   <si>
-    <t>joi1234</t>
-  </si>
-  <si>
     <t>Animais Fantasticos 3</t>
+  </si>
+  <si>
+    <t>Erik</t>
+  </si>
+  <si>
+    <t>erik@email.com</t>
+  </si>
+  <si>
+    <t>Cassiana</t>
+  </si>
+  <si>
+    <t>cassiana@email.com</t>
+  </si>
+  <si>
+    <t>Helena</t>
+  </si>
+  <si>
+    <t>helena@email.com</t>
+  </si>
+  <si>
+    <t>Roberto</t>
+  </si>
+  <si>
+    <t>rob@email.com</t>
   </si>
 </sst>
 </file>
@@ -444,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -459,30 +453,46 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -770,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,53 +806,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="K1" s="17" t="s">
+      <c r="I1" s="21"/>
+      <c r="K1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="17"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="16" t="s">
         <v>6</v>
       </c>
     </row>
@@ -850,17 +860,17 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>67</v>
+      <c r="B3" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="31">
+        <v>123456</v>
       </c>
       <c r="E3" s="10">
-        <v>37365</v>
+        <v>36190</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -882,20 +892,20 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="B4" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="31">
         <v>123456</v>
       </c>
       <c r="E4" s="10">
-        <v>36292</v>
+        <v>34151</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="3">
         <v>2</v>
@@ -914,17 +924,17 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="2">
-        <v>654321</v>
+      <c r="B5" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="31">
+        <v>123456</v>
       </c>
       <c r="E5" s="10">
-        <v>36760</v>
+        <v>35649</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -946,14 +956,14 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>92</v>
+      <c r="B6" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="31">
+        <v>3110</v>
       </c>
       <c r="E6" s="10">
         <v>38376</v>
@@ -972,20 +982,20 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>61</v>
+      <c r="B7" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E7" s="10">
-        <v>37890</v>
+        <v>37365</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -993,48 +1003,48 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D8" s="2">
-        <v>123123456</v>
+        <v>123456</v>
       </c>
       <c r="E8" s="10">
-        <v>35503</v>
+        <v>36292</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="J8" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="18"/>
+      <c r="J8" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="20"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D9" s="2">
-        <v>123456</v>
+        <v>654321</v>
       </c>
       <c r="E9" s="10">
-        <v>33970</v>
+        <v>36760</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="17" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1055,16 +1065,16 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="A12" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
       <c r="J12" s="5">
         <v>3</v>
       </c>
@@ -1073,28 +1083,28 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="19" t="s">
         <v>14</v>
       </c>
       <c r="J13" s="5">
@@ -1109,10 +1119,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>21</v>
@@ -1144,7 +1154,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>24</v>
@@ -1176,7 +1186,7 @@
         <v>26</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>27</v>
@@ -1205,10 +1215,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>29</v>
@@ -1231,10 +1241,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>31</v>
@@ -1252,10 +1262,10 @@
         <v>1</v>
       </c>
       <c r="I18" s="12"/>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K18" s="19"/>
+      <c r="K18" s="23"/>
       <c r="L18" s="12"/>
       <c r="M18" s="13"/>
       <c r="N18" s="12"/>
@@ -1265,10 +1275,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>43</v>
@@ -1285,10 +1295,10 @@
       <c r="H19" s="7">
         <v>1</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="K19" s="24" t="s">
+      <c r="K19" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1300,7 +1310,7 @@
         <v>38</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>39</v>
@@ -1332,7 +1342,7 @@
         <v>40</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>41</v>
@@ -1361,10 +1371,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>49</v>
@@ -1396,7 +1406,7 @@
         <v>44</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>45</v>
@@ -1425,10 +1435,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>47</v>
@@ -1457,10 +1467,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>49</v>
@@ -1489,10 +1499,10 @@
         <v>13</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>50</v>
@@ -1521,10 +1531,10 @@
         <v>14</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>51</v>
@@ -1556,7 +1566,7 @@
         <v>52</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>47</v>
@@ -1579,6 +1589,18 @@
       <c r="K28" s="4">
         <v>8</v>
       </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="26"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="26"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="26"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1590,13 +1612,13 @@
     <mergeCell ref="A12:H12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{F6DA789E-7A62-443C-8583-9B0617688F3B}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{AE005541-B916-4B0F-A20C-7F960508D604}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{276E2BF7-1F89-454C-9F79-B0BC8B7A77A0}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{974A7B58-C928-4380-A45E-C83C0C4653C9}"/>
-    <hyperlink ref="C7" r:id="rId5" xr:uid="{122A6304-3220-474C-AC79-804BE4043433}"/>
-    <hyperlink ref="C8" r:id="rId6" xr:uid="{111A5BC1-31E8-4C45-B587-FA4595D512EA}"/>
-    <hyperlink ref="C9" r:id="rId7" xr:uid="{7FC2B0DF-5C79-40E6-B970-0CFB4A841066}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{62ABD7AB-5E8D-4BE0-9AF9-73869250C8DC}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{DE789DC2-3DEC-42C5-851A-288442FE3249}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{0E107DAD-4238-4716-BBF7-62BD80EE0DFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fim do DDL, DML, DQL e desenvolvimento da documentacao
</commit_message>
<xml_diff>
--- a/OpFlix/MER/M_Diagrama_RaulScapin_Fisico.xlsx
+++ b/OpFlix/MER/M_Diagrama_RaulScapin_Fisico.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20348"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF851327-2DEE-4934-B86D-FD7307702DB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E272A1D-F5B0-47DD-8FED-9011A1CE2331}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
   <si>
     <t>Usuarios</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>rob@email.com</t>
+  </si>
+  <si>
+    <t>Classificacao</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -433,12 +439,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -459,24 +496,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -493,6 +512,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -502,8 +545,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEAC8C8"/>
       <color rgb="FFD25A5A"/>
-      <color rgb="FFEAC8C8"/>
     </mruColors>
   </colors>
   <extLst>
@@ -783,7 +826,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +834,7 @@
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
@@ -799,30 +842,30 @@
     <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="K1" s="24" t="s">
+      <c r="I1" s="27"/>
+      <c r="K1" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="24"/>
+      <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -831,7 +874,7 @@
       <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="14" t="s">
@@ -860,13 +903,13 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="25">
         <v>123456</v>
       </c>
       <c r="E3" s="10">
@@ -892,13 +935,13 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="25">
         <v>123456</v>
       </c>
       <c r="E4" s="10">
@@ -924,13 +967,13 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="25">
         <v>123456</v>
       </c>
       <c r="E5" s="10">
@@ -956,13 +999,13 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="25">
         <v>3110</v>
       </c>
       <c r="E6" s="10">
@@ -982,7 +1025,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="22" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -1017,10 +1060,10 @@
       <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="J8" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="20"/>
+      <c r="K8" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -1041,44 +1084,45 @@
       <c r="F9" s="2">
         <v>0</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="K9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="L9" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J10" s="5">
-        <v>1</v>
-      </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="5">
+        <v>1</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J11" s="5">
-        <v>2</v>
-      </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="5">
+        <v>2</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="J12" s="5">
+      <c r="A12" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
+      <c r="K12" s="5">
         <v>3</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1107,10 +1151,13 @@
       <c r="H13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="5">
+      <c r="I13" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="5">
         <v>4</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1139,10 +1186,13 @@
       <c r="H14" s="7">
         <v>1</v>
       </c>
-      <c r="J14" s="5">
+      <c r="I14" s="7">
+        <v>12</v>
+      </c>
+      <c r="K14" s="5">
         <v>5</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1171,10 +1221,13 @@
       <c r="H15" s="7">
         <v>1</v>
       </c>
-      <c r="J15" s="5">
+      <c r="I15" s="7">
+        <v>12</v>
+      </c>
+      <c r="K15" s="5">
         <v>6</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1203,10 +1256,13 @@
       <c r="H16" s="7">
         <v>2</v>
       </c>
-      <c r="J16" s="5">
+      <c r="I16" s="7">
+        <v>12</v>
+      </c>
+      <c r="K16" s="5">
         <v>7</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1235,6 +1291,9 @@
       <c r="H17" s="7">
         <v>1</v>
       </c>
+      <c r="I17" s="7">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
@@ -1261,12 +1320,13 @@
       <c r="H18" s="7">
         <v>1</v>
       </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="23" t="s">
+      <c r="I18" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="K18" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="K18" s="23"/>
-      <c r="L18" s="12"/>
+      <c r="L18" s="29"/>
       <c r="M18" s="13"/>
       <c r="N18" s="12"/>
     </row>
@@ -1295,10 +1355,13 @@
       <c r="H19" s="7">
         <v>1</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="I19" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="K19" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="L19" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1327,10 +1390,13 @@
       <c r="H20" s="7">
         <v>2</v>
       </c>
-      <c r="J20" s="4">
+      <c r="I20" s="7">
+        <v>12</v>
+      </c>
+      <c r="K20" s="4">
         <v>5</v>
       </c>
-      <c r="K20" s="4">
+      <c r="L20" s="4">
         <v>5</v>
       </c>
     </row>
@@ -1359,10 +1425,13 @@
       <c r="H21" s="7">
         <v>2</v>
       </c>
-      <c r="J21" s="4">
+      <c r="I21" s="7">
+        <v>16</v>
+      </c>
+      <c r="K21" s="4">
         <v>5</v>
       </c>
-      <c r="K21" s="4">
+      <c r="L21" s="4">
         <v>6</v>
       </c>
     </row>
@@ -1391,10 +1460,13 @@
       <c r="H22" s="7">
         <v>1</v>
       </c>
-      <c r="J22" s="4">
-        <v>2</v>
+      <c r="I22" s="7">
+        <v>12</v>
       </c>
       <c r="K22" s="4">
+        <v>2</v>
+      </c>
+      <c r="L22" s="4">
         <v>1</v>
       </c>
     </row>
@@ -1423,10 +1495,13 @@
       <c r="H23" s="7">
         <v>1</v>
       </c>
-      <c r="J23" s="4">
-        <v>2</v>
+      <c r="I23" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="K23" s="4">
+        <v>2</v>
+      </c>
+      <c r="L23" s="4">
         <v>4</v>
       </c>
     </row>
@@ -1455,10 +1530,13 @@
       <c r="H24" s="7">
         <v>1</v>
       </c>
-      <c r="J24" s="4">
+      <c r="I24" s="7">
+        <v>12</v>
+      </c>
+      <c r="K24" s="4">
         <v>4</v>
       </c>
-      <c r="K24" s="4">
+      <c r="L24" s="4">
         <v>9</v>
       </c>
     </row>
@@ -1487,10 +1565,13 @@
       <c r="H25" s="7">
         <v>1</v>
       </c>
-      <c r="J25" s="4">
+      <c r="I25" s="7">
+        <v>12</v>
+      </c>
+      <c r="K25" s="4">
         <v>6</v>
       </c>
-      <c r="K25" s="4">
+      <c r="L25" s="4">
         <v>11</v>
       </c>
     </row>
@@ -1519,10 +1600,13 @@
       <c r="H26" s="7">
         <v>1</v>
       </c>
-      <c r="J26" s="4">
+      <c r="I26" s="7">
+        <v>12</v>
+      </c>
+      <c r="K26" s="4">
         <v>6</v>
       </c>
-      <c r="K26" s="4">
+      <c r="L26" s="4">
         <v>12</v>
       </c>
     </row>
@@ -1551,10 +1635,13 @@
       <c r="H27" s="7">
         <v>1</v>
       </c>
-      <c r="J27" s="4">
+      <c r="I27" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="K27" s="4">
         <v>7</v>
       </c>
-      <c r="K27" s="4">
+      <c r="L27" s="4">
         <v>15</v>
       </c>
     </row>
@@ -1583,33 +1670,36 @@
       <c r="H28" s="7">
         <v>1</v>
       </c>
-      <c r="J28" s="4">
+      <c r="I28" s="7">
+        <v>12</v>
+      </c>
+      <c r="K28" s="4">
         <v>7</v>
       </c>
-      <c r="K28" s="4">
+      <c r="L28" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="26"/>
+      <c r="E35" s="20"/>
     </row>
     <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="26"/>
+      <c r="E36" s="20"/>
     </row>
     <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="26"/>
+      <c r="E37" s="20"/>
     </row>
     <row r="38" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E38" s="26"/>
+      <c r="E38" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="K8:L8"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="K18:L18"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A12:I12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>